<commit_message>
Added TWR error handling
</commit_message>
<xml_diff>
--- a/EngineDataSheet.xlsx
+++ b/EngineDataSheet.xlsx
@@ -5,17 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathi\Desktop\python\PythonSim\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathi\OneDrive\Desktop\Folders\PythonSim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6E04494-8D47-4658-95F7-D0602A59B4D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C703189B-B942-4228-B2EF-6440A8A28520}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18480" yWindow="660" windowWidth="16080" windowHeight="14805" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15300" yWindow="675" windowWidth="12315" windowHeight="14055" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="D12" sheetId="1" r:id="rId1"/>
     <sheet name="F15" sheetId="2" r:id="rId2"/>
     <sheet name="H13" sheetId="3" r:id="rId3"/>
+    <sheet name="E12" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -102,6 +103,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>85936</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>76750</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{673F7B32-0FEF-9F70-C2C7-D8056624F626}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2228850" y="323850"/>
+          <a:ext cx="1514686" cy="3943900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -369,7 +419,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
@@ -1412,4 +1462,19 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0255C950-A47B-479C-9572-25AC3DD97264}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fString improvements, added E engine
</commit_message>
<xml_diff>
--- a/EngineDataSheet.xlsx
+++ b/EngineDataSheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathi\OneDrive\Desktop\Folders\PythonSim\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathi\Desktop\python\PythonSim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C703189B-B942-4228-B2EF-6440A8A28520}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{935AEA65-9231-4994-962C-B5F2BB18E2D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15300" yWindow="675" windowWidth="12315" windowHeight="14055" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="D12" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="6">
   <si>
     <t>Time (s)</t>
   </si>
@@ -51,6 +51,12 @@
   </si>
   <si>
     <t>Upper Time Bound</t>
+  </si>
+  <si>
+    <t>time (s)</t>
+  </si>
+  <si>
+    <t>Upper Limit</t>
   </si>
 </sst>
 </file>
@@ -103,55 +109,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>400050</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>85936</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>76750</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{673F7B32-0FEF-9F70-C2C7-D8056624F626}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2228850" y="323850"/>
-          <a:ext cx="1514686" cy="3943900"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1466,15 +1423,461 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0255C950-A47B-479C-9572-25AC3DD97264}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="D3" sqref="D3:E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="10.5703125" customWidth="1"/>
+    <col min="4" max="4" width="13" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2E-3</v>
+      </c>
+      <c r="B2">
+        <v>1.6779999999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0.05</v>
+      </c>
+      <c r="B3">
+        <v>4.4589999999999996</v>
+      </c>
+      <c r="D3">
+        <v>57.937499999999993</v>
+      </c>
+      <c r="E3">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>0.1</v>
+      </c>
+      <c r="B4">
+        <v>10.430999999999999</v>
+      </c>
+      <c r="D4">
+        <v>119.43999999999998</v>
+      </c>
+      <c r="E4">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>0.2</v>
+      </c>
+      <c r="B5">
+        <v>24.152000000000001</v>
+      </c>
+      <c r="D5">
+        <v>137.21</v>
+      </c>
+      <c r="E5">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>0.27400000000000002</v>
+      </c>
+      <c r="B6">
+        <v>31.959</v>
+      </c>
+      <c r="D6">
+        <v>105.49999999999997</v>
+      </c>
+      <c r="E6">
+        <v>0.27400000000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>0.29199999999999998</v>
+      </c>
+      <c r="B7">
+        <v>32.701999999999998</v>
+      </c>
+      <c r="D7">
+        <v>41.277777777777786</v>
+      </c>
+      <c r="E7">
+        <v>0.29199999999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>0.31</v>
+      </c>
+      <c r="B8">
+        <v>27.957000000000001</v>
+      </c>
+      <c r="D8">
+        <v>-263.61111111111074</v>
+      </c>
+      <c r="E8">
+        <v>0.31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>0.32</v>
+      </c>
+      <c r="B9">
+        <v>25.957000000000001</v>
+      </c>
+      <c r="D9">
+        <v>-199.99999999999983</v>
+      </c>
+      <c r="E9">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>0.33</v>
+      </c>
+      <c r="B10">
+        <v>22.856999999999999</v>
+      </c>
+      <c r="D10">
+        <v>-309.99999999999989</v>
+      </c>
+      <c r="E10">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>0.34</v>
+      </c>
+      <c r="B11">
+        <v>19.128</v>
+      </c>
+      <c r="D11">
+        <v>-372.89999999999958</v>
+      </c>
+      <c r="E11">
+        <v>0.34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>0.35</v>
+      </c>
+      <c r="B12">
+        <v>16.454999999999998</v>
+      </c>
+      <c r="D12">
+        <v>-267.30000000000143</v>
+      </c>
+      <c r="E12">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>0.36</v>
+      </c>
+      <c r="B13">
+        <v>15.314</v>
+      </c>
+      <c r="D13">
+        <v>-114.09999999999972</v>
+      </c>
+      <c r="E13">
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>0.38</v>
+      </c>
+      <c r="B14">
+        <v>13.853</v>
+      </c>
+      <c r="D14">
+        <v>-73.049999999999955</v>
+      </c>
+      <c r="E14">
+        <v>0.38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>0.39</v>
+      </c>
+      <c r="B15">
+        <v>13.436</v>
+      </c>
+      <c r="D15">
+        <v>-41.699999999999946</v>
+      </c>
+      <c r="E15">
+        <v>0.39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>0.4</v>
+      </c>
+      <c r="B16">
+        <v>13.271000000000001</v>
+      </c>
+      <c r="D16">
+        <v>-16.499999999999901</v>
+      </c>
+      <c r="E16">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>0.45</v>
+      </c>
+      <c r="B17">
+        <v>12.07</v>
+      </c>
+      <c r="D17">
+        <v>-24.020000000000017</v>
+      </c>
+      <c r="E17">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>0.5</v>
+      </c>
+      <c r="B18">
+        <v>11.522</v>
+      </c>
+      <c r="D18">
+        <v>-10.960000000000003</v>
+      </c>
+      <c r="E18">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="B19">
+        <v>11.266</v>
+      </c>
+      <c r="D19">
+        <v>-5.12</v>
+      </c>
+      <c r="E19">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>0.6</v>
+      </c>
+      <c r="B20">
+        <v>10.736000000000001</v>
+      </c>
+      <c r="D20">
+        <v>-10.600000000000001</v>
+      </c>
+      <c r="E20">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>0.65</v>
+      </c>
+      <c r="B21">
+        <v>10.776999999999999</v>
+      </c>
+      <c r="D21">
+        <v>0.81999999999997109</v>
+      </c>
+      <c r="E21">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>0.7</v>
+      </c>
+      <c r="B22">
+        <v>10.276</v>
+      </c>
+      <c r="D22">
+        <v>-10.020000000000003</v>
+      </c>
+      <c r="E22">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>0.8</v>
+      </c>
+      <c r="B23">
+        <v>10.105</v>
+      </c>
+      <c r="D23">
+        <v>-1.7099999999999922</v>
+      </c>
+      <c r="E23">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>0.9</v>
+      </c>
+      <c r="B24">
+        <v>9.92</v>
+      </c>
+      <c r="D24">
+        <v>-1.8500000000000054</v>
+      </c>
+      <c r="E24">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>1</v>
+      </c>
+      <c r="B25">
+        <v>9.6929999999999996</v>
+      </c>
+      <c r="D25">
+        <v>-2.2700000000000036</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>1.31</v>
+      </c>
+      <c r="B26">
+        <v>9.7590000000000003</v>
+      </c>
+      <c r="D26">
+        <v>0.21290322580645391</v>
+      </c>
+      <c r="E26">
+        <v>1.31</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>1.3160000000000001</v>
+      </c>
+      <c r="B27">
+        <v>10.696</v>
+      </c>
+      <c r="D27">
+        <v>156.16666666666643</v>
+      </c>
+      <c r="E27">
+        <v>1.3160000000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>1.33</v>
+      </c>
+      <c r="B28">
+        <v>9.6280000000000001</v>
+      </c>
+      <c r="D28">
+        <v>-76.285714285714192</v>
+      </c>
+      <c r="E28">
+        <v>1.33</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>2.38</v>
+      </c>
+      <c r="B29">
+        <v>9.8699999999999992</v>
+      </c>
+      <c r="D29">
+        <v>0.23047619047618967</v>
+      </c>
+      <c r="E29">
+        <v>2.38</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>2.4</v>
+      </c>
+      <c r="B30">
+        <v>6.4420000000000002</v>
+      </c>
+      <c r="D30">
+        <v>-171.39999999999981</v>
+      </c>
+      <c r="E30">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>2.42</v>
+      </c>
+      <c r="B31">
+        <v>3.6739999999999999</v>
+      </c>
+      <c r="D31">
+        <v>-138.39999999999989</v>
+      </c>
+      <c r="E31">
+        <v>2.42</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>2.44</v>
+      </c>
+      <c r="B32">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>-183.69999999999985</v>
+      </c>
+      <c r="E32">
+        <v>2.44</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>